<commit_message>
Added '10' below '9' on sheet 3.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\ExcelProjectTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\Current\ExcelProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,26 +371,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -401,26 +401,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>6</v>
       </c>
@@ -431,28 +431,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="C7:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a '10' in sheet 3.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\ExcelProjectTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\Current\ExcelProjectTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,31 +379,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>0</v>
       </c>
@@ -414,26 +414,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>6</v>
       </c>
@@ -444,28 +444,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="C7:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>